<commit_message>
added new interface; added working joint FISH and single cell dataTables
</commit_message>
<xml_diff>
--- a/testDat/SKY-Daniel_EM_dp_mod_1_tab.xlsx
+++ b/testDat/SKY-Daniel_EM_dp_mod_1_tab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="1380" windowWidth="28800" windowHeight="15940"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="26" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Chr. No.</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>HCT116 Cells</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -177,9 +186,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -509,12 +524,24 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -552,8 +579,8 @@
       <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
+      <c r="F6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -573,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -583,8 +610,8 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
-        <v>2</v>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
@@ -612,8 +639,8 @@
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1">
-        <v>2</v>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -623,8 +650,8 @@
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
-        <v>2</v>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
@@ -692,8 +719,8 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>28</v>
+      <c r="F13" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -710,7 +737,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
@@ -720,20 +747,20 @@
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>30</v>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -749,28 +776,28 @@
       <c r="D16" s="1">
         <v>2</v>
       </c>
-      <c r="E16" s="1">
-        <v>2</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
+      <c r="E16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="1">
-        <v>2</v>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="D17" s="1">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2</v>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F17" s="1">
         <v>2</v>
@@ -790,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1">
         <v>2</v>
@@ -800,20 +827,20 @@
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1">
-        <v>2</v>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="1">
-        <v>2</v>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -840,57 +867,57 @@
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>31</v>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>2</v>
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E22" s="1">
         <v>2</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>32</v>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -949,11 +976,11 @@
       <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="1">
-        <v>2</v>
-      </c>
-      <c r="F26" s="1">
-        <v>2</v>
+      <c r="E26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -981,19 +1008,19 @@
         <v>20</v>
       </c>
       <c r="B28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1027,6 +1054,9 @@
       <c r="F30" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="B7:G28">
+    <sortCondition ref="G7:G28"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added working version of aneuvis based on GA's feedback
</commit_message>
<xml_diff>
--- a/testDat/SKY-Daniel_EM_dp_mod_1_tab.xlsx
+++ b/testDat/SKY-Daniel_EM_dp_mod_1_tab.xlsx
@@ -128,9 +128,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>2,t(1;12;4)</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>2,t(16;11)</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
@@ -662,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -810,19 +810,19 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -890,19 +890,19 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -990,16 +990,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>

</xml_diff>